<commit_message>
add agent attribution feature
</commit_message>
<xml_diff>
--- a/Backend/app/static/facture_cdm.xlsx
+++ b/Backend/app/static/facture_cdm.xlsx
@@ -103,7 +103,7 @@
     <t xml:space="preserve">N° COMPTE :</t>
   </si>
   <si>
-    <t xml:space="preserve">022 780 000 426 003 292 566 174</t>
+    <t xml:space="preserve">021780000014303007029868</t>
   </si>
 </sst>
 </file>
@@ -638,9 +638,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>16200</xdr:colOff>
+      <xdr:colOff>15840</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>15480</xdr:rowOff>
+      <xdr:rowOff>15120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -649,8 +649,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4701240" y="957240"/>
-          <a:ext cx="2472840" cy="601200"/>
+          <a:off x="4701960" y="957240"/>
+          <a:ext cx="2472120" cy="600840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -667,7 +667,7 @@
         <a:fontRef idx="minor"/>
       </xdr:style>
       <xdr:txBody>
-        <a:bodyPr anchor="b">
+        <a:bodyPr lIns="90000" rIns="90000" tIns="45000" bIns="45000" anchor="b">
           <a:noAutofit/>
         </a:bodyPr>
         <a:p>
@@ -703,9 +703,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>801360</xdr:colOff>
+      <xdr:colOff>801000</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>113040</xdr:rowOff>
+      <xdr:rowOff>112680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -714,8 +714,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9555840" y="1008360"/>
-          <a:ext cx="2998080" cy="133560"/>
+          <a:off x="9556560" y="1008360"/>
+          <a:ext cx="2997720" cy="133200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -798,9 +798,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1017000</xdr:colOff>
+      <xdr:colOff>1016640</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>122760</xdr:rowOff>
+      <xdr:rowOff>122400</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -809,8 +809,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9291240" y="1022040"/>
-          <a:ext cx="143280" cy="129600"/>
+          <a:off x="9291960" y="1022040"/>
+          <a:ext cx="142920" cy="129240"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -883,7 +883,7 @@
           </a:pathLst>
         </a:custGeom>
         <a:solidFill>
-          <a:schemeClr val="tx1"/>
+          <a:srgbClr val="ffffff"/>
         </a:solidFill>
         <a:ln w="79375">
           <a:noFill/>
@@ -915,9 +915,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>95400</xdr:colOff>
+      <xdr:colOff>95040</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>207720</xdr:rowOff>
+      <xdr:rowOff>207360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -926,8 +926,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9542520" y="493200"/>
-          <a:ext cx="2305440" cy="133560"/>
+          <a:off x="9543240" y="493200"/>
+          <a:ext cx="2305080" cy="133200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -980,9 +980,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1023480</xdr:colOff>
+      <xdr:colOff>1023120</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>5040</xdr:rowOff>
+      <xdr:rowOff>4680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -991,8 +991,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9238320" y="547200"/>
-          <a:ext cx="202680" cy="86400"/>
+          <a:off x="9239040" y="547200"/>
+          <a:ext cx="202320" cy="86040"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -1119,9 +1119,9 @@
           </a:pathLst>
         </a:custGeom>
         <a:solidFill>
-          <a:schemeClr val="tx1"/>
+          <a:srgbClr val="ffffff"/>
         </a:solidFill>
-        <a:ln>
+        <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </xdr:spPr>
@@ -1151,9 +1151,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1037520</xdr:colOff>
+      <xdr:colOff>1037160</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>166680</xdr:rowOff>
+      <xdr:rowOff>166320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1162,8 +1162,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9238320" y="227520"/>
-          <a:ext cx="216720" cy="129600"/>
+          <a:off x="9239040" y="227520"/>
+          <a:ext cx="216360" cy="129240"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -1327,9 +1327,9 @@
           </a:pathLst>
         </a:custGeom>
         <a:solidFill>
-          <a:schemeClr val="tx1"/>
+          <a:srgbClr val="ffffff"/>
         </a:solidFill>
-        <a:ln>
+        <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </xdr:spPr>
@@ -1359,9 +1359,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1133280</xdr:colOff>
+      <xdr:colOff>1132920</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>136800</xdr:rowOff>
+      <xdr:rowOff>136440</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1370,8 +1370,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9526320" y="193680"/>
-          <a:ext cx="1803240" cy="133560"/>
+          <a:off x="9527040" y="193680"/>
+          <a:ext cx="1802880" cy="133200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1424,9 +1424,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>79200</xdr:colOff>
+      <xdr:colOff>78840</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>46440</xdr:rowOff>
+      <xdr:rowOff>46080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1435,8 +1435,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9558360" y="750960"/>
-          <a:ext cx="2273400" cy="133560"/>
+          <a:off x="9559080" y="750960"/>
+          <a:ext cx="2273040" cy="133200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1483,15 +1483,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>820800</xdr:colOff>
+      <xdr:colOff>820080</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>144000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1040400</xdr:colOff>
+      <xdr:colOff>1039320</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>64080</xdr:rowOff>
+      <xdr:rowOff>63720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1501,7 +1501,7 @@
       <xdr:spPr>
         <a:xfrm flipH="1">
           <a:off x="9238320" y="772560"/>
-          <a:ext cx="219600" cy="129600"/>
+          <a:ext cx="219240" cy="129240"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -1879,7 +1879,7 @@
           </a:pathLst>
         </a:custGeom>
         <a:solidFill>
-          <a:schemeClr val="tx1"/>
+          <a:srgbClr val="ffffff"/>
         </a:solidFill>
         <a:ln w="9525">
           <a:noFill/>
@@ -1903,9 +1903,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>496800</xdr:colOff>
+      <xdr:colOff>496440</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>174240</xdr:rowOff>
+      <xdr:rowOff>173880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1919,7 +1919,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="387000" y="226080"/>
-          <a:ext cx="2450880" cy="367200"/>
+          <a:ext cx="2451240" cy="366840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1941,8 +1941,8 @@
   </sheetPr>
   <dimension ref="A2:J36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="96" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I9" activeCellId="0" sqref="I9"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>